<commit_message>
Sale forecast + sentiment dashboard
</commit_message>
<xml_diff>
--- a/salesForecasting/Accidents.xlsx
+++ b/salesForecasting/Accidents.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kohweiling/Documents/Y4S2/FYP/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\John\Desktop\SMU\SMU term6\FYP_BA\w6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBFE67DC-0F0E-F341-AF06-4ED290D515F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{983196D3-43EF-4E2E-8FF5-C8AC1525E854}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="15120" windowHeight="16740" xr2:uid="{3873E662-1CEF-064D-A8EE-EE81A7D8811B}"/>
+    <workbookView xWindow="9900" yWindow="72" windowWidth="12300" windowHeight="12168" xr2:uid="{3873E662-1CEF-064D-A8EE-EE81A7D8811B}"/>
   </bookViews>
   <sheets>
     <sheet name="license" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="84">
   <si>
     <t>All Classes</t>
   </si>
@@ -288,6 +288,9 @@
   </si>
   <si>
     <t>threeA</t>
+  </si>
+  <si>
+    <t>3_and_3A</t>
   </si>
 </sst>
 </file>
@@ -369,7 +372,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -395,9 +398,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -406,6 +406,13 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -721,20 +728,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0441E873-09A6-3A48-A418-BB3C2608CFE3}">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.5" customWidth="1"/>
-    <col min="2" max="2" width="16.1640625" style="1" customWidth="1"/>
-    <col min="3" max="4" width="15.1640625" customWidth="1"/>
+    <col min="2" max="2" width="16.19921875" style="1" customWidth="1"/>
+    <col min="3" max="4" width="15.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -747,8 +754,11 @@
       <c r="D1" s="3" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" s="13" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>2004</v>
       </c>
@@ -761,8 +771,12 @@
       <c r="D2" s="6" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E2" s="14">
+        <f>SUM($C2,$D2)</f>
+        <v>1270985</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>2005</v>
       </c>
@@ -775,8 +789,13 @@
       <c r="D3" s="5">
         <v>6698</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E3" s="14">
+        <f t="shared" ref="E3:E20" si="0">SUM($C3,$D3)</f>
+        <v>1306234</v>
+      </c>
+      <c r="F3" s="12"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>2006</v>
       </c>
@@ -789,8 +808,12 @@
       <c r="D4" s="5">
         <v>10372</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E4" s="14">
+        <f t="shared" si="0"/>
+        <v>1337761</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>2007</v>
       </c>
@@ -803,8 +826,12 @@
       <c r="D5" s="5">
         <v>17061</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E5" s="14">
+        <f t="shared" si="0"/>
+        <v>1366775</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>2008</v>
       </c>
@@ -817,8 +844,12 @@
       <c r="D6" s="5">
         <v>27632</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E6" s="14">
+        <f t="shared" si="0"/>
+        <v>1428896</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>2009</v>
       </c>
@@ -831,8 +862,12 @@
       <c r="D7" s="5">
         <v>40155</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E7" s="14">
+        <f t="shared" si="0"/>
+        <v>1511425</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>2010</v>
       </c>
@@ -845,8 +880,12 @@
       <c r="D8" s="5">
         <v>53967</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E8" s="14">
+        <f t="shared" si="0"/>
+        <v>1599472</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>2011</v>
       </c>
@@ -859,8 +898,12 @@
       <c r="D9" s="5">
         <v>67923</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E9" s="14">
+        <f t="shared" si="0"/>
+        <v>1661543</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>2012</v>
       </c>
@@ -873,8 +916,12 @@
       <c r="D10" s="5">
         <v>80663</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E10" s="14">
+        <f t="shared" si="0"/>
+        <v>1716061</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>2013</v>
       </c>
@@ -887,8 +934,12 @@
       <c r="D11" s="5">
         <v>93939</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E11" s="14">
+        <f t="shared" si="0"/>
+        <v>1778560</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>2014</v>
       </c>
@@ -901,8 +952,12 @@
       <c r="D12" s="5">
         <v>107203</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E12" s="14">
+        <f t="shared" si="0"/>
+        <v>1837972</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <v>2015</v>
       </c>
@@ -915,8 +970,12 @@
       <c r="D13" s="5">
         <v>122201</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E13" s="14">
+        <f t="shared" si="0"/>
+        <v>1901146</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
         <v>2016</v>
       </c>
@@ -929,8 +988,12 @@
       <c r="D14" s="5">
         <v>138299</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E14" s="14">
+        <f t="shared" si="0"/>
+        <v>1935616</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
         <v>2017</v>
       </c>
@@ -943,8 +1006,12 @@
       <c r="D15" s="5">
         <v>154228</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E15" s="14">
+        <f t="shared" si="0"/>
+        <v>1917320</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
         <v>2018</v>
       </c>
@@ -957,8 +1024,12 @@
       <c r="D16" s="5">
         <v>172298</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E16" s="14">
+        <f t="shared" si="0"/>
+        <v>1951061</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="4">
         <v>2019</v>
       </c>
@@ -971,8 +1042,12 @@
       <c r="D17" s="5">
         <v>191923</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E17" s="14">
+        <f t="shared" si="0"/>
+        <v>1981749</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="4">
         <v>2020</v>
       </c>
@@ -985,33 +1060,45 @@
       <c r="D18" s="5">
         <v>207000</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="9">
+      <c r="E18" s="14">
+        <f t="shared" si="0"/>
+        <v>1995003</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="4">
         <v>2021</v>
       </c>
-      <c r="B19" s="10" t="s">
+      <c r="B19" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C19" s="10" t="s">
+      <c r="C19" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D19" s="10" t="s">
+      <c r="D19" s="9" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="9">
+      <c r="E19" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="4">
         <v>2022</v>
       </c>
-      <c r="B20" s="10" t="s">
+      <c r="B20" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C20" s="10" t="s">
+      <c r="C20" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D20" s="10" t="s">
+      <c r="D20" s="9" t="s">
         <v>2</v>
+      </c>
+      <c r="E20" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1027,12 +1114,12 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -1045,7 +1132,7 @@
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>2008</v>
       </c>
@@ -1058,7 +1145,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>2009</v>
       </c>
@@ -1071,7 +1158,7 @@
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>2010</v>
       </c>
@@ -1084,7 +1171,7 @@
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>2011</v>
       </c>
@@ -1097,7 +1184,7 @@
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>2012</v>
       </c>
@@ -1110,7 +1197,7 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>2013</v>
       </c>
@@ -1123,7 +1210,7 @@
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>2014</v>
       </c>
@@ -1136,7 +1223,7 @@
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>2015</v>
       </c>
@@ -1149,7 +1236,7 @@
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>2016</v>
       </c>
@@ -1162,7 +1249,7 @@
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>2017</v>
       </c>
@@ -1175,7 +1262,7 @@
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>2018</v>
       </c>
@@ -1188,7 +1275,7 @@
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <v>2019</v>
       </c>
@@ -1201,7 +1288,7 @@
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
         <v>2020</v>
       </c>
@@ -1214,7 +1301,7 @@
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -1223,7 +1310,7 @@
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -1232,7 +1319,7 @@
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -1241,7 +1328,7 @@
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -1250,7 +1337,7 @@
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -1259,7 +1346,7 @@
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -1268,7 +1355,7 @@
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -1277,7 +1364,7 @@
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -1286,7 +1373,7 @@
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -1295,7 +1382,7 @@
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -1304,7 +1391,7 @@
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -1313,7 +1400,7 @@
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -1322,7 +1409,7 @@
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -1331,7 +1418,7 @@
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -1340,7 +1427,7 @@
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -1349,7 +1436,7 @@
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -1358,7 +1445,7 @@
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -1367,7 +1454,7 @@
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -1376,7 +1463,7 @@
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -1385,7 +1472,7 @@
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
@@ -1394,7 +1481,7 @@
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
@@ -1403,7 +1490,7 @@
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -1412,7 +1499,7 @@
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -1421,7 +1508,7 @@
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -1443,15 +1530,15 @@
       <selection activeCell="C5" sqref="C5:C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.83203125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="20.1640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="21.1640625" style="2" customWidth="1"/>
-    <col min="4" max="7" width="10.83203125" style="2"/>
+    <col min="1" max="1" width="16.796875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="20.19921875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="21.19921875" style="2" customWidth="1"/>
+    <col min="4" max="7" width="10.796875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>6</v>
       </c>
@@ -1462,7 +1549,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
@@ -1473,7 +1560,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
@@ -1484,7 +1571,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
@@ -1495,40 +1582,40 @@
         <v>1770</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B5" s="2">
         <v>645</v>
       </c>
-      <c r="C5" s="12">
+      <c r="C5" s="11">
         <v>5528.37</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="2">
         <v>687</v>
       </c>
-      <c r="C6" s="12">
+      <c r="C6" s="11">
         <v>5528.37</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B7" s="2">
         <v>646</v>
       </c>
-      <c r="C7" s="12">
+      <c r="C7" s="11">
         <v>5528.37</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>15</v>
       </c>
@@ -1539,7 +1626,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>16</v>
       </c>
@@ -1550,7 +1637,7 @@
         <v>1770</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>17</v>
       </c>
@@ -1561,7 +1648,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>18</v>
       </c>
@@ -1572,7 +1659,7 @@
         <v>1870</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>19</v>
       </c>
@@ -1583,7 +1670,7 @@
         <v>18830</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>20</v>
       </c>
@@ -1594,7 +1681,7 @@
         <v>23225.35</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>21</v>
       </c>
@@ -1605,7 +1692,7 @@
         <v>79471</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>22</v>
       </c>
@@ -1616,7 +1703,7 @@
         <v>40499.64</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>23</v>
       </c>
@@ -1627,29 +1714,29 @@
         <v>64598.63</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B17" s="2">
         <v>684</v>
       </c>
-      <c r="C17" s="11">
+      <c r="C17" s="10">
         <v>64748.74</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B18" s="2">
         <v>695</v>
       </c>
-      <c r="C18" s="11">
+      <c r="C18" s="10">
         <v>157603.07999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>26</v>
       </c>
@@ -1660,7 +1747,7 @@
         <v>176821.55</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>27</v>
       </c>
@@ -1671,7 +1758,7 @@
         <v>179037.35</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>28</v>
       </c>
@@ -1682,7 +1769,7 @@
         <v>160838.56</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>29</v>
       </c>
@@ -1693,7 +1780,7 @@
         <v>101588.46</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>30</v>
       </c>
@@ -1704,7 +1791,7 @@
         <v>109867.09</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>31</v>
       </c>
@@ -1715,7 +1802,7 @@
         <v>141000.35999999999</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>32</v>
       </c>
@@ -1726,7 +1813,7 @@
         <v>131052.86</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>33</v>
       </c>
@@ -1737,7 +1824,7 @@
         <v>108602.3</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>34</v>
       </c>
@@ -1748,7 +1835,7 @@
         <v>88774.36</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>35</v>
       </c>
@@ -1759,7 +1846,7 @@
         <v>169803.64</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>36</v>
       </c>
@@ -1770,7 +1857,7 @@
         <v>117368.75</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>37</v>
       </c>
@@ -1781,18 +1868,18 @@
         <v>102707.44</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>38</v>
       </c>
       <c r="B31" s="2">
         <v>636</v>
       </c>
-      <c r="C31" s="11">
+      <c r="C31" s="10">
         <v>103197.2</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>39</v>
       </c>
@@ -1803,84 +1890,84 @@
         <v>137013.17000000001</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>40</v>
       </c>
       <c r="B33" s="2">
         <v>663</v>
       </c>
-      <c r="C33" s="11">
+      <c r="C33" s="10">
         <v>130645.43</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>41</v>
       </c>
       <c r="B34" s="2">
         <v>629</v>
       </c>
-      <c r="C34" s="11">
+      <c r="C34" s="10">
         <v>141423.82</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>42</v>
       </c>
       <c r="B35" s="2">
         <v>619</v>
       </c>
-      <c r="C35" s="11">
+      <c r="C35" s="10">
         <v>120089.53</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B36" s="2">
         <v>686</v>
       </c>
-      <c r="C36" s="11">
+      <c r="C36" s="10">
         <v>140187.18</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B37" s="2">
         <v>652</v>
       </c>
-      <c r="C37" s="11">
+      <c r="C37" s="10">
         <v>151797.23000000001</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>45</v>
       </c>
       <c r="B38" s="2">
         <v>713</v>
       </c>
-      <c r="C38" s="11">
+      <c r="C38" s="10">
         <v>178628.84</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>46</v>
       </c>
       <c r="B39" s="2">
         <v>618</v>
       </c>
-      <c r="C39" s="11">
+      <c r="C39" s="10">
         <v>93124.51</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>47</v>
       </c>
@@ -1891,29 +1978,29 @@
         <v>80376.28</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>48</v>
       </c>
       <c r="B41" s="2">
         <v>648</v>
       </c>
-      <c r="C41" s="11">
+      <c r="C41" s="10">
         <v>78928.14</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B42" s="2">
         <v>614</v>
       </c>
-      <c r="C42" s="11">
+      <c r="C42" s="10">
         <v>68503.12</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>50</v>
       </c>
@@ -1924,7 +2011,7 @@
         <v>90534.58</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>51</v>
       </c>
@@ -1935,7 +2022,7 @@
         <v>90712.36</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>52</v>
       </c>
@@ -1946,18 +2033,18 @@
         <v>77561.929999999993</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>53</v>
       </c>
       <c r="B46" s="2">
         <v>618</v>
       </c>
-      <c r="C46" s="11">
+      <c r="C46" s="10">
         <v>87770.13</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>54</v>
       </c>
@@ -1968,7 +2055,7 @@
         <v>96235.1</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>56</v>
       </c>
@@ -1979,7 +2066,7 @@
         <v>66084.820000000007</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>55</v>
       </c>
@@ -1990,18 +2077,18 @@
         <v>98937.79</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>57</v>
       </c>
       <c r="B50" s="2">
         <v>677</v>
       </c>
-      <c r="C50" s="11">
+      <c r="C50" s="10">
         <v>128673.9</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>58</v>
       </c>
@@ -2012,18 +2099,18 @@
         <v>54255.96</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>59</v>
       </c>
       <c r="B52" s="2">
         <v>624</v>
       </c>
-      <c r="C52" s="11">
+      <c r="C52" s="10">
         <v>86778.43</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>60</v>
       </c>
@@ -2034,18 +2121,18 @@
         <v>102873.93</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>61</v>
       </c>
       <c r="B54" s="2">
         <v>660</v>
       </c>
-      <c r="C54" s="11">
+      <c r="C54" s="10">
         <v>97540.54</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>62</v>
       </c>
@@ -2056,29 +2143,29 @@
         <v>73344.59</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>63</v>
       </c>
       <c r="B56" s="2">
         <v>687</v>
       </c>
-      <c r="C56" s="11">
+      <c r="C56" s="10">
         <v>119768.12</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>64</v>
       </c>
       <c r="B57" s="2">
         <v>622</v>
       </c>
-      <c r="C57" s="11">
+      <c r="C57" s="10">
         <v>119748.24</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>65</v>
       </c>
@@ -2089,18 +2176,18 @@
         <v>114466.01</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>66</v>
       </c>
       <c r="B59" s="2">
         <v>692</v>
       </c>
-      <c r="C59" s="11">
+      <c r="C59" s="10">
         <v>107960.81</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
         <v>67</v>
       </c>
@@ -2111,7 +2198,7 @@
         <v>119858.32</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>68</v>
       </c>
@@ -2122,7 +2209,7 @@
         <v>108545.53</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>69</v>
       </c>
@@ -2133,7 +2220,7 @@
         <v>102663.47</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
         <v>70</v>
       </c>
@@ -2144,7 +2231,7 @@
         <v>79875.360000000102</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>71</v>
       </c>
@@ -2155,7 +2242,7 @@
         <v>121276.92</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>80</v>
       </c>
@@ -2166,7 +2253,7 @@
         <v>61666.58</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>72</v>
       </c>
@@ -2177,7 +2264,7 @@
         <v>64744.89</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>73</v>
       </c>
@@ -2188,7 +2275,7 @@
         <v>99116.29</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
         <v>74</v>
       </c>
@@ -2199,7 +2286,7 @@
         <v>125336.29</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
         <v>75</v>
       </c>
@@ -2210,7 +2297,7 @@
         <v>110542.11</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
         <v>76</v>
       </c>
@@ -2221,7 +2308,7 @@
         <v>100429.62</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>77</v>
       </c>
@@ -2232,7 +2319,7 @@
         <v>100753.84</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>78</v>
       </c>
@@ -2243,14 +2330,14 @@
         <v>111262.41</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
         <v>79</v>
       </c>
       <c r="B73" s="2">
         <v>588</v>
       </c>
-      <c r="C73" s="11">
+      <c r="C73" s="10">
         <v>135060.34</v>
       </c>
     </row>
@@ -2267,14 +2354,14 @@
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="2"/>
-    <col min="2" max="2" width="20.33203125" style="2" customWidth="1"/>
-    <col min="3" max="5" width="10.83203125" style="2"/>
+    <col min="1" max="1" width="10.796875" style="2"/>
+    <col min="2" max="2" width="20.296875" style="2" customWidth="1"/>
+    <col min="3" max="5" width="10.796875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>4</v>
       </c>
@@ -2282,7 +2369,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="7">
         <v>2004</v>
       </c>
@@ -2290,7 +2377,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="7">
         <v>2005</v>
       </c>
@@ -2298,7 +2385,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="7">
         <v>2006</v>
       </c>
@@ -2306,7 +2393,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="7">
         <v>2007</v>
       </c>
@@ -2314,7 +2401,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="7">
         <v>2008</v>
       </c>
@@ -2322,7 +2409,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="7">
         <v>2009</v>
       </c>
@@ -2330,7 +2417,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="7">
         <v>2010</v>
       </c>
@@ -2338,7 +2425,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="7">
         <v>2011</v>
       </c>
@@ -2346,7 +2433,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="7">
         <v>2012</v>
       </c>
@@ -2354,7 +2441,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="7">
         <v>2013</v>
       </c>
@@ -2362,7 +2449,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="7">
         <v>2014</v>
       </c>
@@ -2370,7 +2457,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="7">
         <v>2015</v>
       </c>
@@ -2378,7 +2465,7 @@
         <v>49755.35</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="7">
         <v>2016</v>
       </c>
@@ -2386,7 +2473,7 @@
         <v>1407127.32</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="7">
         <v>2017</v>
       </c>
@@ -2394,7 +2481,7 @@
         <v>1511610.05</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="7">
         <v>2018</v>
       </c>
@@ -2402,7 +2489,7 @@
         <v>1107397.6000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="7">
         <v>2019</v>
       </c>
@@ -2410,7 +2497,7 @@
         <v>1233814.3799999999</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="7">
         <v>2020</v>
       </c>
@@ -2418,7 +2505,7 @@
         <v>1212728.1200000001</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="7">
         <v>2021</v>
       </c>
@@ -2426,7 +2513,7 @@
         <v>1340885.52</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="7">
         <v>2022</v>
       </c>
@@ -2434,19 +2521,19 @@
         <v>894542.9</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="7"/>
       <c r="B21" s="7"/>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="7"/>
       <c r="B22" s="7"/>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="7"/>
       <c r="B23" s="7"/>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="7"/>
       <c r="B24" s="7"/>
     </row>

</xml_diff>